<commit_message>
add BBW ZZ data
</commit_message>
<xml_diff>
--- a/report/CornTempRes.xlsx
+++ b/report/CornTempRes.xlsx
@@ -269,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0&quot;万吨&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +315,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -503,7 +511,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -620,6 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,6 +674,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -947,8 +957,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1427224000"/>
-        <c:axId val="1427219104"/>
+        <c:axId val="-989290624"/>
+        <c:axId val="-989291168"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1269,11 +1279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1427218016"/>
-        <c:axId val="1427228352"/>
+        <c:axId val="-1431074800"/>
+        <c:axId val="-989291712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1427218016"/>
+        <c:axId val="-1431074800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1323,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427228352"/>
+        <c:crossAx val="-989291712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1321,7 +1331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1427228352"/>
+        <c:axId val="-989291712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,12 +1379,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427218016"/>
+        <c:crossAx val="-1431074800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1427219104"/>
+        <c:axId val="-989291168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,12 +1418,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427224000"/>
+        <c:crossAx val="-989290624"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="1427224000"/>
+        <c:axId val="-989290624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1427219104"/>
+        <c:crossAx val="-989291168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1761,8 +1771,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1427229984"/>
-        <c:axId val="1427229440"/>
+        <c:axId val="-949150368"/>
+        <c:axId val="-949153088"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2077,11 +2087,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1427228896"/>
-        <c:axId val="1427220192"/>
+        <c:axId val="-949156352"/>
+        <c:axId val="-949146560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1427228896"/>
+        <c:axId val="-949156352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2121,7 +2131,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427220192"/>
+        <c:crossAx val="-949146560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2129,7 +2139,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1427220192"/>
+        <c:axId val="-949146560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2177,12 +2187,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427228896"/>
+        <c:crossAx val="-949156352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1427229440"/>
+        <c:axId val="-949153088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2216,12 +2226,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427229984"/>
+        <c:crossAx val="-949150368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1427229984"/>
+        <c:axId val="-949150368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1427229440"/>
+        <c:crossAx val="-949153088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2576,8 +2586,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1427220736"/>
-        <c:axId val="1427217472"/>
+        <c:axId val="-949157984"/>
+        <c:axId val="-949151456"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2898,11 +2908,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1427224544"/>
-        <c:axId val="1427216928"/>
+        <c:axId val="-949148736"/>
+        <c:axId val="-949152000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1427224544"/>
+        <c:axId val="-949148736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2942,7 +2952,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427216928"/>
+        <c:crossAx val="-949152000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2950,7 +2960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1427216928"/>
+        <c:axId val="-949152000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,12 +3008,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427224544"/>
+        <c:crossAx val="-949148736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1427217472"/>
+        <c:axId val="-949151456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,12 +3047,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1427220736"/>
+        <c:crossAx val="-949157984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="1427220736"/>
+        <c:axId val="-949157984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,7 +3062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1427217472"/>
+        <c:crossAx val="-949151456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3396,8 +3406,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1509462592"/>
-        <c:axId val="1509458784"/>
+        <c:axId val="-949153632"/>
+        <c:axId val="-949161248"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3718,11 +3728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1324020016"/>
-        <c:axId val="1509450624"/>
+        <c:axId val="-949152544"/>
+        <c:axId val="-949148192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1324020016"/>
+        <c:axId val="-949152544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3762,7 +3772,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1509450624"/>
+        <c:crossAx val="-949148192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3770,7 +3780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1509450624"/>
+        <c:axId val="-949148192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3818,12 +3828,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1324020016"/>
+        <c:crossAx val="-949152544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1509458784"/>
+        <c:axId val="-949161248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3857,12 +3867,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1509462592"/>
+        <c:crossAx val="-949153632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1509462592"/>
+        <c:axId val="-949153632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3872,7 +3882,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1509458784"/>
+        <c:crossAx val="-949161248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -6228,7 +6238,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="3067050" y="4295775"/>
-          <a:ext cx="7200014" cy="4310476"/>
+          <a:ext cx="7285739" cy="4310476"/>
           <a:chOff x="3095625" y="4295775"/>
           <a:chExt cx="7209989" cy="5052012"/>
         </a:xfrm>
@@ -6992,8 +7002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AY21" sqref="AY21:BD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7047,144 +7057,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.15">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="40"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55">
+      <c r="E1" s="55"/>
+      <c r="F1" s="56">
         <v>2014</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="50">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="51">
         <v>2015</v>
       </c>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
-      <c r="AH1" s="50"/>
-      <c r="AI1" s="50"/>
-      <c r="AJ1" s="50"/>
-      <c r="AK1" s="50"/>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="50"/>
-      <c r="AO1" s="50"/>
-      <c r="AP1" s="50"/>
-      <c r="AQ1" s="50"/>
-      <c r="AR1" s="50"/>
-      <c r="AS1" s="50"/>
-      <c r="AT1" s="50"/>
-      <c r="AU1" s="50"/>
-      <c r="AV1" s="50"/>
-      <c r="AW1" s="50"/>
-      <c r="AX1" s="50"/>
-      <c r="AY1" s="50"/>
-      <c r="AZ1" s="50"/>
-      <c r="BA1" s="50"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.15">
-      <c r="A2" s="52"/>
-      <c r="B2" s="51"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="52"/>
       <c r="C2" s="40"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="56" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="58" t="s">
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="59" t="s">
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="56" t="s">
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="57" t="s">
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="AK2" s="57"/>
-      <c r="AL2" s="57"/>
-      <c r="AM2" s="57"/>
-      <c r="AN2" s="57"/>
-      <c r="AO2" s="57"/>
-      <c r="AP2" s="58" t="s">
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AQ2" s="58"/>
-      <c r="AR2" s="58"/>
-      <c r="AS2" s="58"/>
-      <c r="AT2" s="58"/>
-      <c r="AU2" s="58"/>
-      <c r="AV2" s="59" t="s">
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="59"/>
+      <c r="AS2" s="59"/>
+      <c r="AT2" s="59"/>
+      <c r="AU2" s="59"/>
+      <c r="AV2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="AW2" s="59"/>
-      <c r="AX2" s="59"/>
-      <c r="AY2" s="59"/>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="59"/>
+      <c r="AW2" s="60"/>
+      <c r="AX2" s="60"/>
+      <c r="AY2" s="60"/>
+      <c r="AZ2" s="60"/>
+      <c r="BA2" s="60"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.15">
-      <c r="A3" s="52"/>
-      <c r="B3" s="51"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="40" t="s">
         <v>50</v>
       </c>
@@ -9701,10 +9711,10 @@
       <c r="X17" s="7">
         <v>5307700</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="50">
         <v>95929</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="50">
         <v>1507</v>
       </c>
       <c r="AA17" s="12">
@@ -9841,10 +9851,10 @@
       <c r="L18" s="7">
         <v>12562000</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="4">
         <v>103384</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="4">
         <v>1559</v>
       </c>
       <c r="O18" s="12">
@@ -9861,10 +9871,10 @@
       <c r="R18" s="7">
         <v>3358700</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18">
         <v>25000</v>
       </c>
-      <c r="T18" s="8">
+      <c r="T18">
         <v>1606</v>
       </c>
       <c r="U18" s="12">
@@ -9881,10 +9891,10 @@
       <c r="X18" s="7">
         <v>5307700</v>
       </c>
-      <c r="Y18" s="8">
+      <c r="Y18" s="50">
         <v>37038</v>
       </c>
-      <c r="Z18" s="8">
+      <c r="Z18" s="50">
         <v>1422</v>
       </c>
       <c r="AA18" s="12">
@@ -9901,10 +9911,10 @@
       <c r="AD18" s="10">
         <v>45620000</v>
       </c>
-      <c r="AE18" s="8">
+      <c r="AE18">
         <v>544343</v>
       </c>
-      <c r="AF18" s="8">
+      <c r="AF18">
         <v>1461</v>
       </c>
       <c r="AG18" s="12">
@@ -9921,10 +9931,10 @@
       <c r="AJ18" s="7">
         <v>44510000</v>
       </c>
-      <c r="AK18" s="8">
+      <c r="AK18" s="4">
         <v>1942502</v>
       </c>
-      <c r="AL18" s="8">
+      <c r="AL18" s="4">
         <v>1542</v>
       </c>
       <c r="AM18" s="12">
@@ -9941,10 +9951,10 @@
       <c r="AP18" s="7">
         <v>11240000</v>
       </c>
-      <c r="AQ18" s="8">
+      <c r="AQ18" s="4">
         <v>463673</v>
       </c>
-      <c r="AR18" s="8">
+      <c r="AR18" s="4">
         <v>1617</v>
       </c>
       <c r="AS18" s="12">
@@ -9961,10 +9971,10 @@
       <c r="AV18" s="7">
         <v>21060000</v>
       </c>
-      <c r="AW18" s="8">
+      <c r="AW18" s="4">
         <v>649607</v>
       </c>
-      <c r="AX18" s="8">
+      <c r="AX18" s="4">
         <v>1564</v>
       </c>
       <c r="AY18" s="12">
@@ -10021,10 +10031,10 @@
       <c r="L19" s="7">
         <v>12562000</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M19" s="4">
         <v>35294</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="4">
         <v>1607</v>
       </c>
       <c r="O19" s="12">
@@ -10072,10 +10082,10 @@
       <c r="AD19" s="10">
         <v>45620000</v>
       </c>
-      <c r="AE19" s="8">
+      <c r="AE19">
         <v>1119354</v>
       </c>
-      <c r="AF19" s="8">
+      <c r="AF19">
         <v>1477</v>
       </c>
       <c r="AG19" s="12">
@@ -10092,10 +10102,10 @@
       <c r="AJ19" s="7">
         <v>44510000</v>
       </c>
-      <c r="AK19" s="8">
+      <c r="AK19" s="4">
         <v>2424081</v>
       </c>
-      <c r="AL19" s="8">
+      <c r="AL19" s="4">
         <v>1568</v>
       </c>
       <c r="AM19" s="12">
@@ -10112,10 +10122,10 @@
       <c r="AP19" s="7">
         <v>11240000</v>
       </c>
-      <c r="AQ19" s="8">
+      <c r="AQ19" s="4">
         <v>494698</v>
       </c>
-      <c r="AR19" s="8">
+      <c r="AR19" s="4">
         <v>1679</v>
       </c>
       <c r="AS19" s="12">
@@ -10132,10 +10142,10 @@
       <c r="AV19" s="7">
         <v>21060000</v>
       </c>
-      <c r="AW19" s="8">
+      <c r="AW19" s="4">
         <v>920781</v>
       </c>
-      <c r="AX19" s="8">
+      <c r="AX19" s="4">
         <v>1571</v>
       </c>
       <c r="AY19" s="12">
@@ -10418,10 +10428,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E10:M22"/>
+  <dimension ref="E10:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10432,12 +10442,13 @@
     <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="5:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="5:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="5:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F11" s="14">
         <f>INDEX(detail!A4:A99999,COUNTA(detail!$B$4:$B$99999))</f>
         <v>43398</v>
@@ -10465,12 +10476,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="5:13" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="5:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="E12">
         <f>I12+I17</f>
         <v>1692230</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="65">
         <v>2014</v>
       </c>
       <c r="G12" s="18" t="s">
@@ -10500,13 +10511,17 @@
         <f>INDEX(detail!K4:K99999,COUNTA(detail!$B4:$B99999))/10000</f>
         <v>420.8759</v>
       </c>
+      <c r="N12" s="66">
+        <f>L12+L17</f>
+        <v>3690.79</v>
+      </c>
     </row>
-    <row r="13" spans="5:13" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="5:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="E13">
         <f>I13+I18</f>
         <v>2459375</v>
       </c>
-      <c r="F13" s="64"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="18" t="s">
         <v>2</v>
       </c>
@@ -10534,13 +10549,17 @@
         <f>INDEX(detail!Q4:Q99999,COUNTA(detail!$B$4:$B$99999))/10000</f>
         <v>0.72540000000000004</v>
       </c>
+      <c r="N13" s="66">
+        <f t="shared" ref="N13:N15" si="0">L13+L18</f>
+        <v>3829.5637999999999</v>
+      </c>
     </row>
-    <row r="14" spans="5:13" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="5:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="E14">
         <f>I14+I19</f>
         <v>494698</v>
       </c>
-      <c r="F14" s="64"/>
+      <c r="F14" s="65"/>
       <c r="G14" s="18" t="s">
         <v>3</v>
       </c>
@@ -10568,13 +10587,17 @@
         <f>INDEX(detail!W4:W99999,COUNTA(detail!$B$4:$B$99999))/10000</f>
         <v>1.7310000000000001</v>
       </c>
+      <c r="N14" s="66">
+        <f t="shared" si="0"/>
+        <v>1007.879</v>
+      </c>
     </row>
-    <row r="15" spans="5:13" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="5:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="E15">
         <f>I15+I20</f>
         <v>967091</v>
       </c>
-      <c r="F15" s="64"/>
+      <c r="F15" s="65"/>
       <c r="G15" s="18" t="s">
         <v>16</v>
       </c>
@@ -10602,33 +10625,37 @@
         <f>INDEX(detail!AC4:AC99999,COUNTA(detail!$B$4:$B$99999))/10000</f>
         <v>0.27660000000000001</v>
       </c>
+      <c r="N15" s="66">
+        <f t="shared" si="0"/>
+        <v>1428.2611999999999</v>
+      </c>
     </row>
-    <row r="16" spans="5:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F16" s="60" t="s">
+    <row r="16" spans="5:14" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="F16" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="61"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="22">
         <f>SUM(H12:H15)</f>
         <v>5261.9501</v>
       </c>
       <c r="I16" s="23">
-        <f t="shared" ref="I16:M16" si="0">SUM(I12:I15)</f>
+        <f t="shared" ref="I16:M16" si="1">SUM(I12:I15)</f>
         <v>654480</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
       <c r="L16" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4838.3411999999998</v>
       </c>
       <c r="M16" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>423.60889999999995</v>
       </c>
     </row>
     <row r="17" spans="6:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F17" s="64">
+      <c r="F17" s="65">
         <v>2015</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -10660,7 +10687,7 @@
       </c>
     </row>
     <row r="18" spans="6:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F18" s="64"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="18" t="s">
         <v>2</v>
       </c>
@@ -10690,7 +10717,7 @@
       </c>
     </row>
     <row r="19" spans="6:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F19" s="64"/>
+      <c r="F19" s="65"/>
       <c r="G19" s="18" t="s">
         <v>3</v>
       </c>
@@ -10720,7 +10747,7 @@
       </c>
     </row>
     <row r="20" spans="6:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F20" s="64"/>
+      <c r="F20" s="65"/>
       <c r="G20" s="18" t="s">
         <v>16</v>
       </c>
@@ -10750,50 +10777,50 @@
       </c>
     </row>
     <row r="21" spans="6:13" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="61"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="22">
         <f>SUM(H17:H20)</f>
         <v>12243</v>
       </c>
       <c r="I21" s="23">
-        <f t="shared" ref="I21:M21" si="1">SUM(I17:I20)</f>
+        <f t="shared" ref="I21:M21" si="2">SUM(I17:I20)</f>
         <v>4958914</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
       <c r="L21" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5118.1527999999998</v>
       </c>
       <c r="M21" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7124.8472000000002</v>
       </c>
     </row>
     <row r="22" spans="6:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="62" t="s">
+      <c r="F22" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="63"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="26">
         <f>H16+H21</f>
         <v>17504.950100000002</v>
       </c>
       <c r="I22" s="27">
-        <f t="shared" ref="I22:M22" si="2">I16+I21</f>
+        <f t="shared" ref="I22:M22" si="3">I16+I21</f>
         <v>5613394</v>
       </c>
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
       <c r="L22" s="26">
-        <f>L16+L21+56</f>
-        <v>10012.493999999999</v>
+        <f>L16+L21+58</f>
+        <v>10014.493999999999</v>
       </c>
       <c r="M22" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7548.4561000000003</v>
       </c>
     </row>

</xml_diff>